<commit_message>
Excel feature and UploadDataToDB
</commit_message>
<xml_diff>
--- a/Credentials/Credentials.xlsx
+++ b/Credentials/Credentials.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>database credentaials</t>
   </si>
@@ -140,6 +140,21 @@
   </si>
   <si>
     <t>["name"]</t>
+  </si>
+  <si>
+    <t>table_creation_sql_query</t>
+  </si>
+  <si>
+    <t>table_name</t>
+  </si>
+  <si>
+    <t>etl</t>
+  </si>
+  <si>
+    <t>insertedData</t>
+  </si>
+  <si>
+    <t>CREATE TABLE insertedData (Id INT , empid INT, name VARCHAR(255), designation VARCHAR(255))</t>
   </si>
 </sst>
 </file>
@@ -184,9 +199,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -762,7 +780,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,7 +810,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -806,7 +824,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
@@ -817,7 +835,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
@@ -860,13 +878,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -918,28 +940,44 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>14</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>$A$28:$A$31</formula1>
+      <formula1>$A$29:$A$32</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>

<commit_message>
Remove column A and generate data of different rows
</commit_message>
<xml_diff>
--- a/Credentials/Credentials.xlsx
+++ b/Credentials/Credentials.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Source" sheetId="2" r:id="rId2"/>
-    <sheet name="Target" sheetId="3" r:id="rId3"/>
-    <sheet name="Checks" sheetId="5" r:id="rId4"/>
-    <sheet name="UploadDataToDB" sheetId="4" r:id="rId5"/>
+    <sheet name="Source" sheetId="2" r:id="rId1"/>
+    <sheet name="Target" sheetId="3" r:id="rId2"/>
+    <sheet name="Checks" sheetId="5" r:id="rId3"/>
+    <sheet name="UploadDataToDB" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
-  <si>
-    <t>database credentaials</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>user</t>
   </si>
@@ -40,12 +36,6 @@
     <t xml:space="preserve">database </t>
   </si>
   <si>
-    <t>source_file_to_upload_in_db</t>
-  </si>
-  <si>
-    <t>target_file</t>
-  </si>
-  <si>
     <t>root</t>
   </si>
   <si>
@@ -56,9 +46,6 @@
   </si>
   <si>
     <t>myempdb</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> C:\Users\prashant.sahu\Downloads\SourceData.csv</t>
   </si>
   <si>
     <t>C:\Users\prashant.sahu\Downloads\TargetData.csv</t>
@@ -486,85 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,83 +487,191 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>$A$28:$A$31</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView zoomScale="86" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -669,117 +689,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
-  <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>$A$28:$A$31</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -793,76 +705,76 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -892,86 +804,86 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>